<commit_message>
add okr and dkr
</commit_message>
<xml_diff>
--- a/AppData/Reports/ExamGradesSheet/Template.xlsx
+++ b/AppData/Reports/ExamGradesSheet/Template.xlsx
@@ -18,15 +18,93 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Главное управление по образованию Брестского облисполкома
+Учреждение образования
+«Пинский государственный профессионально-технический колледж легкой промышленности»</t>
+  </si>
+  <si>
+    <t>ЭКЗАМЕНАЦИОННАЯ ВЕДОМОСТЬ</t>
+  </si>
+  <si>
+    <t>(очная форма получения образования)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Учебная цисциплина </t>
+  </si>
+  <si>
+    <t>Основы алгоритмизации и программирование</t>
+  </si>
+  <si>
+    <t>Курс</t>
+  </si>
+  <si>
+    <t>учебная группа</t>
+  </si>
+  <si>
+    <t>Т191-19</t>
+  </si>
+  <si>
+    <t>Специальность</t>
+  </si>
+  <si>
+    <t>2-40 01 01 Программное обеспечение информационных технологий</t>
+  </si>
+  <si>
+    <t>Преподаватель</t>
+  </si>
+  <si>
+    <t>Аргер Надежда Викторовна</t>
+  </si>
+  <si>
+    <t>№ п/п</t>
+  </si>
+  <si>
+    <t>ФИО</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -45,15 +123,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +202,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +242,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +282,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -331,12 +464,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="10" width="9.5703125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ExamGradesSheet finish testing, improve validation
</commit_message>
<xml_diff>
--- a/AppData/Reports/ExamGradesSheet/Template.xlsx
+++ b/AppData/Reports/ExamGradesSheet/Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>№ п/п</t>
   </si>
@@ -488,40 +488,7 @@
     <t>{SemesterGrade}</t>
   </si>
   <si>
-    <t>{ExamGrade} ({ExamGradeText})</t>
-  </si>
-  <si>
-    <t>Курс или семетр</t>
-  </si>
-  <si>
-    <t>Последний семестр</t>
-  </si>
-  <si>
-    <t>Курсовой проект</t>
-  </si>
-  <si>
-    <t>Может ли быть 2 на 1 курс</t>
-  </si>
-  <si>
-    <t>Что делать с учащимися если убыл или пришел</t>
-  </si>
-  <si>
-    <t>Курсовая работа на курс только 1 - 0</t>
-  </si>
-  <si>
-    <t>Выбранный семестр</t>
-  </si>
-  <si>
-    <t>Оценка по экзамену с текущего семестра</t>
-  </si>
-  <si>
-    <t>Перечень учащихся привязан к текущему семестру</t>
-  </si>
-  <si>
-    <t>за 2 семестра если 2 семестр и только за 1 если для первого семестра</t>
-  </si>
-  <si>
-    <t>!!! Валидация</t>
+    <t>{ExamGrade}</t>
   </si>
 </sst>
 </file>
@@ -596,18 +563,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -704,8 +665,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -986,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1007,7 +968,7 @@
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
@@ -1021,7 +982,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +996,7 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1049,8 +1010,8 @@
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
@@ -1098,7 +1059,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1130,7 +1091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1156,8 +1117,8 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -1171,7 +1132,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1148,7 @@
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -1203,7 +1164,7 @@
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1180,7 @@
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1233,7 +1194,7 @@
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1246,11 +1207,8 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="N15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1263,9 +1221,6 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="N16" s="2" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1280,12 +1235,6 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="N17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="18" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1318,9 +1267,6 @@
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
-      <c r="N19" s="2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="20" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -1378,82 +1324,314 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
     </row>
     <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="N25" s="21" t="s">
-        <v>45</v>
-      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F31" s="21" t="s">
-        <v>43</v>
-      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="I32" s="21" t="s">
-        <v>44</v>
-      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>